<commit_message>
dataset actulizados(no todos),grafico del matias (histograma)
</commit_message>
<xml_diff>
--- a/dataset/region/sexo_edad_antofagasta.xlsx
+++ b/dataset/region/sexo_edad_antofagasta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirit\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfurn\Desktop\proyectovdd\errores\dashboard_seguridad\dataset\region\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25AD767F-C8C3-4709-AC22-7F27FFAFE15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8029A39-9EFA-4CF4-A4EB-71BA0456CC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A7839AC3-B251-4F49-A43B-BD219A9DCD71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7839AC3-B251-4F49-A43B-BD219A9DCD71}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -181,28 +181,28 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -521,13 +521,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8623EC-4125-44E1-92EB-80C845ABDB4D}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W54" sqref="W53:W54"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +590,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -655,7 +655,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -720,7 +720,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -785,7 +785,7 @@
         <v>4424</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -850,7 +850,7 @@
         <v>6273</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -915,7 +915,7 @@
         <v>3371</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -980,7 +980,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>15469</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>4293</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>7806</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>5318</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>3</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>19148</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>3</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>8717</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>3</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>14079</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>8689</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>3</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>3</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>3</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>34617</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>15</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>15</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>15</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>15</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>15</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>15</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>3741</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>15</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>15</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>4549</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>15</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>5767</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>15</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>2257</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>15</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>15</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>15</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>13171</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>15</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>15</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>15</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>5919</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>15</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>7311</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>15</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>2891</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>15</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>15</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>15</v>
       </c>

</xml_diff>